<commit_message>
import cattle sheet prototype completed
</commit_message>
<xml_diff>
--- a/templates/cattle.xlsx
+++ b/templates/cattle.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="27">
   <si>
     <t>Name</t>
   </si>
@@ -72,6 +72,39 @@
   </si>
   <si>
     <t>Officer Livestock</t>
+  </si>
+  <si>
+    <t>Name1</t>
+  </si>
+  <si>
+    <t>Father Name 1</t>
+  </si>
+  <si>
+    <t>Address of affectee</t>
+  </si>
+  <si>
+    <t>Peshawar</t>
+  </si>
+  <si>
+    <t>Some Reason</t>
+  </si>
+  <si>
+    <t>big</t>
+  </si>
+  <si>
+    <t>2015-31-04</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Name2</t>
+  </si>
+  <si>
+    <t>Father Name 2</t>
+  </si>
+  <si>
+    <t>2012-03-02</t>
   </si>
 </sst>
 </file>
@@ -107,8 +140,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -389,18 +423,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" customWidth="1"/>
     <col min="7" max="7" width="21.42578125" customWidth="1"/>
     <col min="8" max="8" width="15" customWidth="1"/>
-    <col min="9" max="9" width="16.85546875" customWidth="1"/>
+    <col min="9" max="9" width="16.85546875" style="1" customWidth="1"/>
     <col min="10" max="10" width="17.5703125" customWidth="1"/>
     <col min="11" max="11" width="14.140625" customWidth="1"/>
     <col min="12" max="12" width="16.140625" customWidth="1"/>
@@ -435,7 +470,7 @@
       <c r="H1" t="s">
         <v>12</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="J1" t="s">
@@ -458,9 +493,110 @@
       </c>
       <c r="P1" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2">
+        <v>12234123</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2">
+        <v>1000</v>
+      </c>
+      <c r="H2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2" t="s">
+        <v>23</v>
+      </c>
+      <c r="O2" t="s">
+        <v>23</v>
+      </c>
+      <c r="P2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3">
+        <v>12234123</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3">
+        <v>1000</v>
+      </c>
+      <c r="H3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P3" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>